<commit_message>
Added Export Data Module
</commit_message>
<xml_diff>
--- a/temp.xlsx
+++ b/temp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AJ2"/>
+  <dimension ref="A1:AJ3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -617,7 +617,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -626,7 +626,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>UTS transverse</t>
+          <t>UTS axial</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -790,6 +790,186 @@
         </is>
       </c>
       <c r="AJ2" t="inlineStr">
+        <is>
+          <t>Test Value 24</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>12</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>A08</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>UTS axial</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Mechanical Properties</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>220 IPHWR</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>RAPS-1</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>10.5</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>07-10-2024</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Test entry</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>Test Value 1</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>Test Value 2</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Test Value 3</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>Test Value 4</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>Test Value 5</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>Test Value 6</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>Test Value 7</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>Test Value 8</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>Test Value 9</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>Test Value 10</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>Test Value 11</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>Test Value 12</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>Test Value 13</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>Test Value 14</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>Test Value 15</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>Test Value 16</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>Test Value 17</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>Test Value 18</t>
+        </is>
+      </c>
+      <c r="AE3" t="inlineStr">
+        <is>
+          <t>Test Value 19</t>
+        </is>
+      </c>
+      <c r="AF3" t="inlineStr">
+        <is>
+          <t>Test Value 20</t>
+        </is>
+      </c>
+      <c r="AG3" t="inlineStr">
+        <is>
+          <t>Test Value 21</t>
+        </is>
+      </c>
+      <c r="AH3" t="inlineStr">
+        <is>
+          <t>Test Value 22</t>
+        </is>
+      </c>
+      <c r="AI3" t="inlineStr">
+        <is>
+          <t>Test Value 23</t>
+        </is>
+      </c>
+      <c r="AJ3" t="inlineStr">
         <is>
           <t>Test Value 24</t>
         </is>

</xml_diff>